<commit_message>
Changed the draw to take into account age
</commit_message>
<xml_diff>
--- a/Templates/BO_3.xlsx
+++ b/Templates/BO_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\winlin\Python\AJDS\Judo-Plus-Sheets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7655E650-8BC1-4483-8BD0-152685F8C61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A356E5-F2C1-4140-9D33-1018D9EAB474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31395" yWindow="4140" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Melhor 3" sheetId="4" r:id="rId1"/>
@@ -87,13 +87,13 @@
     <t>2 Atletas</t>
   </si>
   <si>
-    <t>2013/2012</t>
-  </si>
-  <si>
-    <t>Rio Maior, 19 de Maio de 2024</t>
-  </si>
-  <si>
-    <t>Projecto Judo +  Rio Maior</t>
+    <t>Torres Novas, 5 de Outubro de 2024</t>
+  </si>
+  <si>
+    <t>Escalão:</t>
+  </si>
+  <si>
+    <t>Projecto Judo +  Torres Novas</t>
   </si>
 </sst>
 </file>
@@ -231,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -321,13 +321,11 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -338,7 +336,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -351,7 +349,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -360,124 +358,28 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -497,7 +399,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,14 +407,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -529,10 +428,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -552,7 +447,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -561,7 +455,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -575,56 +469,59 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1099,7 +996,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K4" sqref="K4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,21 +1008,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -1150,7 +1047,7 @@
     </row>
     <row r="3" spans="1:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1171,268 +1068,276 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="50"/>
+      <c r="I4" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="38"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="52"/>
     </row>
     <row r="5" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="55"/>
+      <c r="L5" s="42"/>
       <c r="O5" s="3"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
     </row>
     <row r="6" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="40" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <v>1</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <v>1</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <v>1</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="K6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="3"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
     </row>
     <row r="7" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="29" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="15">
         <v>2</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>2</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <v>2</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="3"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
       <c r="O8" s="3"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="23"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
       <c r="O9" s="3"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
     </row>
     <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
       <c r="O10" s="3"/>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
       <c r="O11" s="3"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
     </row>
     <row r="12" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="46" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="12"/>
       <c r="O12" s="3"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="25"/>
-      <c r="C13" s="43" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="26"/>
-      <c r="H13" s="5" t="s">
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="23"/>
+      <c r="H13" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="18"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="49"/>
       <c r="O13" s="3"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
     </row>
     <row r="14" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="H14" s="17" t="s">
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="H14" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="41"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="28"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="39"/>
       <c r="O14" s="3"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
     </row>
     <row r="15" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
       <c r="O15" s="3"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
     </row>
     <row r="16" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="M16" s="3"/>
     </row>
     <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="7" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="G23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="10"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="9"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="I14:M14"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -1440,12 +1345,7 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I14:K14"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="I13:K13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Bugs Fixed. Features Added. Code structure cleanup
</commit_message>
<xml_diff>
--- a/Templates/BO_3.xlsx
+++ b/Templates/BO_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\winlin\Python\AJDS\Judo-Plus-Sheets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A356E5-F2C1-4140-9D33-1018D9EAB474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B45FF1-A332-41E3-B4D3-FBBCA20FB0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31395" yWindow="4140" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Melhor 3" sheetId="4" r:id="rId1"/>
@@ -399,7 +399,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,6 +484,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -505,23 +514,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -996,7 +993,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:M4"/>
+      <selection activeCell="J4" sqref="J4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,36 +1061,36 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="52"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="51"/>
     </row>
     <row r="5" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="42"/>
+      <c r="L5" s="45"/>
       <c r="O5" s="3"/>
       <c r="Q5" s="32"/>
       <c r="R5" s="32"/>
       <c r="S5" s="32"/>
     </row>
     <row r="6" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1126,9 +1123,9 @@
       <c r="S6" s="31"/>
     </row>
     <row r="7" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="25" t="s">
         <v>6</v>
       </c>
@@ -1197,8 +1194,8 @@
     <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1215,11 +1212,11 @@
     <row r="11" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
@@ -1253,20 +1250,20 @@
     </row>
     <row r="13" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="22"/>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="23"/>
       <c r="H13" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="49"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="42"/>
       <c r="O13" s="3"/>
       <c r="Q13" s="31"/>
       <c r="R13" s="31"/>
@@ -1332,20 +1329,19 @@
       <c r="L23" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="I14:M14"/>
+  <mergeCells count="12">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="J4:M4"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="I14:M14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Draw logic adjusted. Groups up to 10 elements added.
</commit_message>
<xml_diff>
--- a/Templates/BO_3.xlsx
+++ b/Templates/BO_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\winlin\Python\AJDS\Judo-Plus-Sheets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B45FF1-A332-41E3-B4D3-FBBCA20FB0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AD9699-DD2D-4CCE-AF9A-502D2C27AD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Melhor 3" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nº</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>2 Atletas</t>
-  </si>
-  <si>
-    <t>Torres Novas, 5 de Outubro de 2024</t>
   </si>
   <si>
     <t>Escalão:</t>
@@ -399,7 +396,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -475,6 +472,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,13 +484,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -502,22 +505,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1026,7 +1020,7 @@
     </row>
     <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3"/>
       <c r="E2" s="3"/>
@@ -1043,9 +1037,7 @@
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1064,33 +1056,33 @@
     <row r="4" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="I4" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="51"/>
+      <c r="I4" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="38"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="31"/>
     </row>
     <row r="5" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="45"/>
+      <c r="L5" s="47"/>
       <c r="O5" s="3"/>
       <c r="Q5" s="32"/>
       <c r="R5" s="32"/>
       <c r="S5" s="32"/>
     </row>
     <row r="6" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="45" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1123,9 +1115,9 @@
       <c r="S6" s="31"/>
     </row>
     <row r="7" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="25" t="s">
         <v>6</v>
       </c>
@@ -1194,8 +1186,8 @@
     <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1212,11 +1204,11 @@
     <row r="11" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
@@ -1234,14 +1226,14 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="40"/>
       <c r="N12" s="12"/>
       <c r="O12" s="3"/>
       <c r="Q12" s="31"/>
@@ -1250,20 +1242,20 @@
     </row>
     <row r="13" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="22"/>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="23"/>
       <c r="H13" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="42"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="50"/>
       <c r="O13" s="3"/>
       <c r="Q13" s="31"/>
       <c r="R13" s="31"/>
@@ -1275,11 +1267,11 @@
       <c r="H14" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="37"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="39"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="40"/>
       <c r="O14" s="3"/>
       <c r="Q14" s="31"/>
       <c r="R14" s="31"/>
@@ -1330,18 +1322,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="J4:M4"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="J4:M4"/>
     <mergeCell ref="H12:M12"/>
     <mergeCell ref="I13:M13"/>
-    <mergeCell ref="I14:M14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="200" r:id="rId1"/>

</xml_diff>